<commit_message>
fixed segment and powertrain split
</commit_message>
<xml_diff>
--- a/data/Alloys.xlsx
+++ b/data/Alloys.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\7. Students projects\Giulia\Python Scripts\03.07.2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6C8079-8EDC-4192-95E0-CED6BA7208BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D5DF23-3164-4AA2-BC68-871E862FF3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{48DDE29B-6874-4114-BE3F-4619753A6B04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{48DDE29B-6874-4114-BE3F-4619753A6B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -691,20 +691,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859594CF-B80A-4EAA-92A9-C97E6AF1E775}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -722,7 +722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -742,7 +742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -760,7 +760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -782,7 +782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
@@ -804,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -826,7 +826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -846,7 +846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -864,7 +864,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -882,7 +882,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>42</v>
       </c>
@@ -900,7 +900,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -918,7 +918,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
@@ -936,7 +936,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
@@ -954,7 +954,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
@@ -972,7 +972,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -990,7 +990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1014,7 +1014,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>57</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>61</v>
       </c>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>79</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1152,7 +1152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1164,7 +1164,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1184,6 +1184,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1191,16 +1192,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5ACC76-9A98-495E-9830-D981C9EE71C5}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1239,7 +1240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1277,10 +1278,10 @@
         <v>0.85</v>
       </c>
       <c r="M2" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>2.9999999999999992E-2</v>
       </c>
       <c r="F3" s="2">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="G3" s="2">
         <v>0.11999999999999997</v>
@@ -1306,10 +1307,10 @@
         <v>4.4999999999999971E-2</v>
       </c>
       <c r="I3" s="2">
-        <v>0.27</v>
+        <v>0.8</v>
       </c>
       <c r="J3" s="2">
-        <v>0.27</v>
+        <v>0.9</v>
       </c>
       <c r="K3" s="2">
         <v>0.18</v>
@@ -1318,10 +1319,10 @@
         <v>4.5000000000000005E-2</v>
       </c>
       <c r="M3" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>75</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>6.9999999999999979E-2</v>
       </c>
       <c r="F4" s="2">
-        <v>0.63</v>
+        <v>0.8</v>
       </c>
       <c r="G4" s="2">
         <v>0.27999999999999992</v>
@@ -1347,10 +1348,10 @@
         <v>0.10499999999999993</v>
       </c>
       <c r="I4" s="2">
-        <v>0.63</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="2">
-        <v>0.63</v>
+        <v>0</v>
       </c>
       <c r="K4" s="2">
         <v>0.42</v>
@@ -1364,5 +1365,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>